<commit_message>
added aiptw for ate
</commit_message>
<xml_diff>
--- a/Overview of functions.xlsx
+++ b/Overview of functions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Functions</t>
   </si>
@@ -140,29 +140,6 @@
 samp_n_controls (numeric)</t>
   </si>
   <si>
-    <t>Function: an_pweight
-Input: an_data (format as pop)
-    match_weights (numeric vector, same # obs as an_data)
-    samp_weights (numeric vector, same # obs as an_data)
-    estimand ("ate" or "att")
-    metric (string, "rr", "rd"  or "rr")
-    pweight_type (string, e.g. "pweight_ht")
-    g (numeric vector, 3x # obs as an_data--1st n obs are predictions for observed data, 2nd n obs are predictions when A_1=1 for everyone and 3rd n obs are predictions when A_1=0 for everyone)
-Output: est (numeric scalar)</t>
-  </si>
-  <si>
-    <t>Function: an_tmle
-Input: an_data (format as pop)
-    match_weights (numeric vector, same # obs as an_data)
-    samp_weights (numeric vector, same # obs as an_data)
-    covs (string vector, e.g. c("W1 ","W2","W3"))
-    estimand ("ate" or "att")
-    metric (string, "rr", "rd"  or "rr")
-    g (numeric vector, 3x # obs as an_data--1st n obs are predictions for observed data, 2nd n obs are predictions when A_1=1 for everyone and 3rd n obs are predictions when A_1=0 for everyone)
-    q (numeric vector, 3x # obs as an_data--1st n obs are predictions for observed data, 2nd n obs are predictions when A_1=1 for everyone and 3rd n obs are predictions when A_1=0 for everyone)
-Output: est (numeric scalar)</t>
-  </si>
-  <si>
     <t>Function: est_q
 Input: an_data (if the analysis is bcm, this is the full sample, otherwise it is an_data) ,
    match_weights (numeric vector, same obs as an_data),
@@ -258,6 +235,40 @@
         analyses (data frame of all analysis specifications )
 Output: g (data frame of all formulated estimates of the probability of tx-- n rows per method)
 This function calls est_g to estimate the probability of treatment given covariates</t>
+  </si>
+  <si>
+    <t>Function: an_pweight
+Input: an_data (format as pop)
+    match_weights (numeric vector, same # obs as an_data)
+    samp_weights (numeric vector, same # obs as an_data)
+    estimand ("ate" or "att")
+    metric (string, "rr", "rd"  or "rr")
+    pweight_type (string, e.g. "pweight_ht")
+    g (numeric vector, same # obs as an_data, predicted prob of treatment)
+Output: est (numeric scalar)</t>
+  </si>
+  <si>
+    <t>Function: an_aiptw
+Input: an_data (format as pop)
+    samp_weights (numeric vector, same # obs as an_data)
+    covs (string vector, e.g. c("W1 ","W2","W3"))
+    estimand ("ate" or "att")
+    metric (string, "rr", "rd"  or "rr")
+    g (numeric vector, same # obs as an_data, predicted prob of tx)
+    q (numeric vector, 3x # obs as an_data--1st n obs are predictions for observed data, 2nd n obs are predictions when A_1=1 for everyone and 3rd n obs are predictions when A_1=0 for everyone)
+Output: est (numeric scalar)</t>
+  </si>
+  <si>
+    <t>Function: an_tmle
+Input: an_data (format as pop)
+    match_weights (numeric vector, same # obs as an_data)
+    samp_weights (numeric vector, same # obs as an_data)
+    covs (string vector, e.g. c("W1 ","W2","W3"))
+    estimand ("ate" or "att")
+    metric (string, "rr", "rd"  or "rr")
+    g (numeric vector, same # obs as an_data, predicted prob of tx)
+    q (numeric vector, 3x # obs as an_data--1st n obs are predictions for observed data, 2nd n obs are predictions when A_1=1 for everyone and 3rd n obs are predictions when A_1=0 for everyone)
+Output: est (numeric scalar)</t>
   </si>
 </sst>
 </file>
@@ -610,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +693,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -690,7 +701,7 @@
     </row>
     <row r="9" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="165" x14ac:dyDescent="0.25">
@@ -698,26 +709,26 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="240" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="297.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -725,28 +736,33 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="180" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="232.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="186" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" ht="120" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>